<commit_message>
tambahan kode festronik saat export import dokumen
</commit_message>
<xml_diff>
--- a/public/template_limbah_masuk.xlsx
+++ b/public/template_limbah_masuk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\wastelog\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DEAFAB-8DA3-473E-87BB-9FB7A39CACF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B18957-969E-4959-BB6B-A6ECD9D9E9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Tanggal</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Berat (kg)</t>
+  </si>
+  <si>
+    <t>Kode Festronik</t>
   </si>
 </sst>
 </file>
@@ -399,15 +402,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,6 +423,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>